<commit_message>
working on ledger uploads, payment vouchers
</commit_message>
<xml_diff>
--- a/public/templates/ledger_sample_template.xlsx
+++ b/public/templates/ledger_sample_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\work\Downloads\FireShot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aqsa Work\Softlin Tech\newpresence360\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" tabRatio="838"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>S.No</t>
   </si>
@@ -71,13 +71,16 @@
   </si>
   <si>
     <t xml:space="preserve">Investments,Account Receivable </t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,12 +95,6 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FFCE9178"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -156,9 +153,6 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -167,6 +161,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -726,46 +723,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" style="5" customWidth="1"/>
     <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" customWidth="1"/>
-    <col min="40" max="40" width="21" customWidth="1"/>
-    <col min="41" max="41" width="17" customWidth="1"/>
-    <col min="44" max="44" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.8" customHeight="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" ht="22.8" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="19.2" customHeight="1">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
@@ -779,20 +772,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29.4" customHeight="1">
-      <c r="A3" s="5">
+    <row r="3" spans="1:5" ht="29.4" customHeight="1">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>